<commit_message>
new changes in mira.xlsx
</commit_message>
<xml_diff>
--- a/psychology/CBT_new/mira.xlsx
+++ b/psychology/CBT_new/mira.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Искажения" sheetId="1" state="visible" r:id="rId3"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="405">
   <si>
     <t xml:space="preserve">№ позиции</t>
   </si>
@@ -770,6 +770,67 @@
 связи в будущем</t>
   </si>
   <si>
+    <t xml:space="preserve">Любовь не зависит
+от достижений</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Я должен быть лучше,
+чтобы заслужить любовь</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Обсуждение дефицита любви к себе на
+сессии с терапевтом</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Глубокая убеждённость в том, что любовь всегда обусловлена
+достижениями.
+2) Это связано с детским опытом, где внимание и признание
+родителей ощущалось как зависящее от моих успехов.
+3) Этот взгляд усиливает чувство собственной недостаточности,
+приводит к постоянному стремлению к совершенству.
+4) Истощает эмоциональные ресурсы и затрудняет
+построение близких, безусловных отношений.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">убеждённость
+достижения
+детский опыт
+успехи
+собственная недостаточность
+стремление к совершенству
+эмоциональные ресурсы
+близкие отношения</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Прогресс сохраняется
+при продолжении
+терапии</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Я не вижу своего прогресса
+и улучшения состояния</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Обсуждение базовых потребностей и осознание
+большого количества дефицитов</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Склонность оценивать состояние через объективные, чётко
+измеримые показатели, что может вести к недооценке субъективных,
+но значимых изменений.
+2) Такой подход может не только усиливать чувство застоя, но
+и создавать риск потери мотивации, так как
+мелкие, но важные достижения остаются незамеченными.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">объективные показатели
+недооценка изменений
+чувство застоя
+риск потери мотивации
+мелкие достижения
+остаются незамеченными</t>
+  </si>
+  <si>
     <t xml:space="preserve">1</t>
   </si>
   <si>
@@ -813,6 +874,12 @@
   </si>
   <si>
     <t xml:space="preserve">15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17</t>
   </si>
   <si>
     <t xml:space="preserve">Разбор 1 — Навешивание ярлыков | // моя работа по дому //</t>
@@ -1477,6 +1544,125 @@
   <si>
     <t xml:space="preserve">12. Если у вас есть полное право быть достойным любви и принятия, как вы теперь относитесь к первоначальной мысли, что вы "недостаточно хорош, чтобы вас любили и принимали безусловно"?</t>
   </si>
+  <si>
+    <t xml:space="preserve">Разбор 16 — Долженствование | // убежденность, что любовь нужно заслужить //</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Я должен быть лучше, чтобы заслужить любовь</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Любовь не зависит от убеждений</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Какие доказательства есть в пользу того, что вы действительно должны быть лучше, чтобы заслужить любовь?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Что заставляет вас думать, что любовь можно заслужить только через определённые качества, а не просто за то, кто вы есть?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Если в детстве любовь часто связывалась с вашими успехами, означает ли это, что любовь всегда должна быть обусловлена достижениями?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. А как вы думаете, могли ли ваши родители ценить вас не только за успехи, но просто за то, что вы их ребёнок, даже если они не всегда выражали это явно?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5. Если вы сомневаетесь в этом, то как вы объясняете тот факт, что родители всё же оставались рядом с вами, заботились о вас или уделяли вам внимание, даже когда вы не добивались успехов?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6. Если это была лишь обязанность, как вы думаете, могли ли они при этом испытывать к вам чувства, которые не зависели от ваших успехов, даже если они не умели их показать?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7. Но если представить, что кто-то другой, не вы, рос бы в похожих условиях — вы бы сказали, что любовь к нему могла существовать, даже если она выражалась через требования или ожидания?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8. Если любовь всегда обусловлена достижениями, как вы объясните случаи, когда люди любят друг друга, несмотря на их ошибки, слабости или отсутствие успехов?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9. А как вы думаете, почему вам кажется странным, что кто-то может любить другого человека просто за то, какой он есть, а не за его успехи?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10. Если ваш жизненный опыт не включал таких примеров, означает ли это, что такие чувства в принципе не могут существовать?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11. Тогда как вы думаете, если такие чувства всё же существуют, возможно ли, что и вы способны быть любимым просто за то, кто вы есть, а не за то, что вы делаете?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12. Что заставляет вас думать, что способность быть любимым — это что-то, что нужно заслужить или развить, а не то, что уже есть в каждом человеке по своей природе?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13. А есть ли в вашей жизни люди, которые продолжают общаться с вами или быть рядом, даже когда вы не стараетесь что-то доказывать или достигать?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14. Если это так, как вы объясните, почему они продолжают общение не только из чувства долга, но, возможно, ещё и по собственной инициативе, даже когда могли бы этого не делать?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15. Если это всего лишь привычка, то почему, как вы думаете, они выбирают поддерживать именно эту привычку — быть рядом с вами, а не, например, прекратить общение?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16. А если задуматься, возможно ли, что эти «блага» — это не только ваши действия или достижения, но и вы сами: ваша личность, ваши качества, то, как вы есть в их жизни?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17. Если рассмотреть это с этой стороны, как вы думаете, возможно ли, что люди ценят вас не только за то, что вы делаете, но и просто за то, каким вы являетесь для них?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18. Если допустить, что это возможно, как вам кажется, что это меняет в вашем убеждении, что любовь нужно заслуживать, становясь лучше?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19. Если эти сомнения начинают появляться, как вы думаете, что для вас важнее: продолжать верить, что любовь нужно заслуживать, или допустить, что её можно получать просто за то, какой вы есть?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20. И если вы допускаете это, что вы чувствуете по отношению к своему убеждению, что нужно быть лучше, чтобы заслужить любовь?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Разбор 17 — Фильтрация | // прогресс в терапии //</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Я не вижу своего прогресса и
+улучшения состояния</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Прогресс сохраняется при продолжении
+терапии</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Что убеждает вас в том, что вы действительно не видите прогресса или улучшения своего состояния?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Если ощущение ухудшения возникает после сеансов, означает ли это, что прогресса действительно нет, или это может быть частью какого-то процесса, который вы пока не до конца понимаете?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Если это сопротивление изменениям, как вы думаете, может ли оно быть временным явлением, которое не отменяет общий прогресс?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. Если вы допускаете, что это временно, какие признаки, даже самые маленькие, могут свидетельствовать о том, что прогресс всё же есть?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5. Если ваш терапевт замечает ваши усилия и продолжает работать с уверенностью в вашем процессе, может ли это указывать на то, что прогресс виден со стороны, даже если вам пока сложно его ощутить?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6. Что мешает вам заметить этот прогресс с вашей стороны?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7. А какие именно объективные показатели могли бы для вас стать доказательством того, что состояние действительно улучшается?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8. Если пока проблемы обсуждаются с разных сторон, может ли это быть важным шагом для их более глубокого понимания и, как следствие, их постепенного разрешения?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9. Если понимание проблем становится глубже, даже сейчас, разве это не может быть одним из тех самых признаков прогресса, который вы искали?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10. Если это так, как вы теперь смотрите на мысль о том, что вы не видите своего прогресса и улучшения состояния?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11. Что вызывает ваши сомнения в том, что более глубокое понимание проблем может быть прогрессом?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12. Если вы признаёте, что более глубокое понимание проблем — это часть прогресса, можно ли сказать, что ваш прогресс всё же существует, хоть и проявляется не так явно, как вам хотелось бы?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13. Если вы теперь видите, что прогресс есть, даже в его малозаметных проявлениях, как это меняет ваше отношение к первоначальной мысли о том, что вы не видите своего прогресса и улучшения состояния?</t>
+  </si>
 </sst>
 </file>
 
@@ -1486,7 +1672,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1534,18 +1720,6 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1709,7 +1883,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="33">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1839,14 +2013,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2251,10 +2417,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2685,6 +2851,58 @@
         <v>5</v>
       </c>
     </row>
+    <row r="17" customFormat="false" ht="94.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="13" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="14" t="n">
+        <v>45638</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="G17" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="H17" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="94.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="13" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="14" t="n">
+        <v>45638</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="G18" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="H18" s="20" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2701,10 +2919,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L234"/>
+  <dimension ref="A1:L274"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A208" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H238" activeCellId="0" sqref="H238"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2722,54 +2940,58 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="F1" s="24" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="G1" s="24" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="H1" s="24" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="I1" s="24" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="J1" s="24" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="K1" s="24" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="L1" s="24" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="24" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>140</v>
-      </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+        <v>150</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>152</v>
+      </c>
       <c r="F2" s="24"/>
       <c r="G2" s="24"/>
       <c r="H2" s="24"/>
@@ -2862,7 +3084,7 @@
     </row>
     <row r="13" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="25" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="B13" s="25"/>
       <c r="C13" s="25"/>
@@ -2872,7 +3094,7 @@
       <c r="G13" s="25"/>
       <c r="H13" s="25"/>
       <c r="I13" s="24" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2883,7 +3105,7 @@
       <c r="C14" s="26"/>
       <c r="D14" s="26"/>
       <c r="E14" s="27" t="s">
-        <v>143</v>
+        <v>155</v>
       </c>
       <c r="F14" s="27"/>
       <c r="G14" s="27"/>
@@ -2891,52 +3113,52 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="28" t="s">
-        <v>144</v>
+        <v>156</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="28" t="s">
-        <v>145</v>
+        <v>157</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="28" t="s">
-        <v>146</v>
+        <v>158</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="28" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="28" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="28" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="28" t="s">
-        <v>150</v>
+        <v>162</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="28" t="s">
-        <v>151</v>
+        <v>163</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="28" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="25" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
       <c r="B25" s="25"/>
       <c r="C25" s="25"/>
@@ -2946,18 +3168,18 @@
       <c r="G25" s="25"/>
       <c r="H25" s="25"/>
       <c r="I25" s="24" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="26" t="s">
-        <v>154</v>
+        <v>166</v>
       </c>
       <c r="B26" s="26"/>
       <c r="C26" s="26"/>
       <c r="D26" s="26"/>
       <c r="E26" s="27" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="F26" s="27"/>
       <c r="G26" s="27"/>
@@ -2965,57 +3187,57 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="28" t="s">
-        <v>156</v>
+        <v>168</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="28" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="28" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="28" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="28" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="28" t="s">
-        <v>161</v>
+        <v>173</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="28" t="s">
-        <v>162</v>
+        <v>174</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="28" t="s">
-        <v>163</v>
+        <v>175</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="28" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="28" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="25" t="s">
-        <v>166</v>
+        <v>178</v>
       </c>
       <c r="B38" s="25"/>
       <c r="C38" s="25"/>
@@ -3025,18 +3247,18 @@
       <c r="G38" s="25"/>
       <c r="H38" s="25"/>
       <c r="I38" s="24" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="29" t="s">
-        <v>167</v>
+        <v>179</v>
       </c>
       <c r="B39" s="29"/>
       <c r="C39" s="29"/>
       <c r="D39" s="29"/>
       <c r="E39" s="27" t="s">
-        <v>168</v>
+        <v>180</v>
       </c>
       <c r="F39" s="27"/>
       <c r="G39" s="27"/>
@@ -3044,77 +3266,77 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="28" t="s">
-        <v>169</v>
+        <v>181</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="28" t="s">
-        <v>170</v>
+        <v>182</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="28" t="s">
-        <v>171</v>
+        <v>183</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="28" t="s">
-        <v>172</v>
+        <v>184</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="28" t="s">
-        <v>173</v>
+        <v>185</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="28" t="s">
-        <v>174</v>
+        <v>186</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="28" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="28" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="28" t="s">
-        <v>177</v>
+        <v>189</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="28" t="s">
-        <v>178</v>
+        <v>190</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="28" t="s">
-        <v>179</v>
+        <v>191</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="28" t="s">
-        <v>180</v>
+        <v>192</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="28" t="s">
-        <v>181</v>
+        <v>193</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="28" t="s">
-        <v>182</v>
+        <v>194</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="25" t="s">
-        <v>183</v>
+        <v>195</v>
       </c>
       <c r="B55" s="25"/>
       <c r="C55" s="25"/>
@@ -3124,18 +3346,18 @@
       <c r="G55" s="25"/>
       <c r="H55" s="25"/>
       <c r="I55" s="24" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="52.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="29" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="B56" s="29"/>
       <c r="C56" s="29"/>
       <c r="D56" s="29"/>
       <c r="E56" s="27" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="F56" s="27"/>
       <c r="G56" s="27"/>
@@ -3143,62 +3365,62 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="28" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="28" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="28" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="28" t="s">
-        <v>189</v>
+        <v>201</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="28" t="s">
-        <v>190</v>
+        <v>202</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="28" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="28" t="s">
-        <v>192</v>
+        <v>204</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="28" t="s">
-        <v>193</v>
+        <v>205</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="28" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="28" t="s">
-        <v>195</v>
+        <v>207</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="28" t="s">
-        <v>196</v>
+        <v>208</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="25" t="s">
-        <v>197</v>
+        <v>209</v>
       </c>
       <c r="B69" s="25"/>
       <c r="C69" s="25"/>
@@ -3208,7 +3430,7 @@
       <c r="G69" s="25"/>
       <c r="H69" s="25"/>
       <c r="I69" s="24" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="36.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3219,7 +3441,7 @@
       <c r="C70" s="29"/>
       <c r="D70" s="29"/>
       <c r="E70" s="27" t="s">
-        <v>198</v>
+        <v>210</v>
       </c>
       <c r="F70" s="27"/>
       <c r="G70" s="27"/>
@@ -3227,62 +3449,62 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="28" t="s">
-        <v>199</v>
+        <v>211</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="28" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="28" t="s">
-        <v>201</v>
+        <v>213</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="28" t="s">
-        <v>202</v>
+        <v>214</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="28" t="s">
-        <v>203</v>
+        <v>215</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="30" t="s">
-        <v>204</v>
+        <v>216</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="28" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="28" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="28" t="s">
-        <v>207</v>
+        <v>219</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="28" t="s">
-        <v>208</v>
+        <v>220</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="28" t="s">
-        <v>209</v>
+        <v>221</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="25" t="s">
-        <v>210</v>
+        <v>222</v>
       </c>
       <c r="B83" s="25"/>
       <c r="C83" s="25"/>
@@ -3292,7 +3514,7 @@
       <c r="G83" s="25"/>
       <c r="H83" s="25"/>
       <c r="I83" s="24" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3303,7 +3525,7 @@
       <c r="C84" s="29"/>
       <c r="D84" s="29"/>
       <c r="E84" s="27" t="s">
-        <v>211</v>
+        <v>223</v>
       </c>
       <c r="F84" s="27"/>
       <c r="G84" s="27"/>
@@ -3311,52 +3533,52 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="28" t="s">
-        <v>212</v>
+        <v>224</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="28" t="s">
-        <v>213</v>
+        <v>225</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="28" t="s">
-        <v>214</v>
+        <v>226</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="28" t="s">
-        <v>215</v>
+        <v>227</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="28" t="s">
-        <v>216</v>
+        <v>228</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="28" t="s">
-        <v>217</v>
+        <v>229</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="28" t="s">
-        <v>218</v>
+        <v>230</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="28" t="s">
-        <v>219</v>
+        <v>231</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="28" t="s">
-        <v>220</v>
+        <v>232</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="25" t="s">
-        <v>221</v>
+        <v>233</v>
       </c>
       <c r="B95" s="25"/>
       <c r="C95" s="25"/>
@@ -3366,7 +3588,7 @@
       <c r="G95" s="25"/>
       <c r="H95" s="25"/>
       <c r="I95" s="24" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="19.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3385,62 +3607,62 @@
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="28" t="s">
-        <v>222</v>
+        <v>234</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="28" t="s">
-        <v>223</v>
+        <v>235</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="28" t="s">
-        <v>224</v>
+        <v>236</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="28" t="s">
-        <v>225</v>
+        <v>237</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="28" t="s">
-        <v>226</v>
+        <v>238</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="28" t="s">
-        <v>227</v>
+        <v>239</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="28" t="s">
-        <v>228</v>
+        <v>240</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="28" t="s">
-        <v>229</v>
+        <v>241</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="28" t="s">
-        <v>230</v>
+        <v>242</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="28" t="s">
-        <v>231</v>
+        <v>243</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="28" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="25" t="s">
-        <v>233</v>
+        <v>245</v>
       </c>
       <c r="B109" s="25"/>
       <c r="C109" s="25"/>
@@ -3450,7 +3672,7 @@
       <c r="G109" s="25"/>
       <c r="H109" s="25"/>
       <c r="I109" s="24" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="27.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3461,7 +3683,7 @@
       <c r="C110" s="31"/>
       <c r="D110" s="31"/>
       <c r="E110" s="27" t="s">
-        <v>234</v>
+        <v>246</v>
       </c>
       <c r="F110" s="27"/>
       <c r="G110" s="27"/>
@@ -3469,62 +3691,62 @@
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="28" t="s">
-        <v>235</v>
+        <v>247</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="28" t="s">
-        <v>236</v>
+        <v>248</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="28" t="s">
-        <v>237</v>
+        <v>249</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="28" t="s">
-        <v>238</v>
+        <v>250</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="28" t="s">
-        <v>239</v>
+        <v>251</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="28" t="s">
-        <v>240</v>
+        <v>252</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="28" t="s">
-        <v>241</v>
+        <v>253</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="28" t="s">
-        <v>242</v>
+        <v>254</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="28" t="s">
-        <v>243</v>
+        <v>255</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="28" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="28" t="s">
-        <v>245</v>
+        <v>257</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="25" t="s">
-        <v>246</v>
+        <v>258</v>
       </c>
       <c r="B123" s="25"/>
       <c r="C123" s="25"/>
@@ -3534,7 +3756,7 @@
       <c r="G123" s="25"/>
       <c r="H123" s="25"/>
       <c r="I123" s="24" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3545,7 +3767,7 @@
       <c r="C124" s="29"/>
       <c r="D124" s="29"/>
       <c r="E124" s="27" t="s">
-        <v>247</v>
+        <v>259</v>
       </c>
       <c r="F124" s="27"/>
       <c r="G124" s="27"/>
@@ -3553,77 +3775,77 @@
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="28" t="s">
-        <v>248</v>
+        <v>260</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="28" t="s">
-        <v>249</v>
+        <v>261</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="28" t="s">
-        <v>250</v>
+        <v>262</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="28" t="s">
-        <v>251</v>
+        <v>263</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="28" t="s">
-        <v>252</v>
+        <v>264</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="28" t="s">
-        <v>253</v>
+        <v>265</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="28" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="28" t="s">
-        <v>255</v>
+        <v>267</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="28" t="s">
-        <v>256</v>
+        <v>268</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="28" t="s">
-        <v>257</v>
+        <v>269</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="28" t="s">
-        <v>258</v>
+        <v>270</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="28" t="s">
-        <v>259</v>
+        <v>271</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="28" t="s">
-        <v>260</v>
+        <v>272</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="28" t="s">
-        <v>261</v>
+        <v>273</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="25" t="s">
-        <v>262</v>
+        <v>274</v>
       </c>
       <c r="B140" s="25"/>
       <c r="C140" s="25"/>
@@ -3633,7 +3855,7 @@
       <c r="G140" s="25"/>
       <c r="H140" s="25"/>
       <c r="I140" s="24" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3644,7 +3866,7 @@
       <c r="C141" s="29"/>
       <c r="D141" s="29"/>
       <c r="E141" s="27" t="s">
-        <v>263</v>
+        <v>275</v>
       </c>
       <c r="F141" s="27"/>
       <c r="G141" s="27"/>
@@ -3652,82 +3874,82 @@
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="28" t="s">
-        <v>264</v>
+        <v>276</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="28" t="s">
-        <v>265</v>
+        <v>277</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="28" t="s">
-        <v>266</v>
+        <v>278</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="28" t="s">
-        <v>267</v>
+        <v>279</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="28" t="s">
-        <v>268</v>
+        <v>280</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="28" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="28" t="s">
-        <v>270</v>
+        <v>282</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="28" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="28" t="s">
-        <v>272</v>
+        <v>284</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="28" t="s">
-        <v>273</v>
+        <v>285</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="28" t="s">
-        <v>274</v>
+        <v>286</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="28" t="s">
-        <v>275</v>
+        <v>287</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="28" t="s">
-        <v>276</v>
+        <v>288</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="28" t="s">
-        <v>277</v>
+        <v>289</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="28" t="s">
-        <v>278</v>
+        <v>290</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="25" t="s">
-        <v>279</v>
+        <v>291</v>
       </c>
       <c r="B158" s="25"/>
       <c r="C158" s="25"/>
@@ -3737,7 +3959,7 @@
       <c r="G158" s="25"/>
       <c r="H158" s="25"/>
       <c r="I158" s="24" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3748,7 +3970,7 @@
       <c r="C159" s="29"/>
       <c r="D159" s="29"/>
       <c r="E159" s="27" t="s">
-        <v>280</v>
+        <v>292</v>
       </c>
       <c r="F159" s="27"/>
       <c r="G159" s="27"/>
@@ -3756,72 +3978,72 @@
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="28" t="s">
-        <v>281</v>
+        <v>293</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="28" t="s">
-        <v>282</v>
+        <v>294</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="28" t="s">
-        <v>283</v>
+        <v>295</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="28" t="s">
-        <v>284</v>
+        <v>296</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="28" t="s">
-        <v>285</v>
+        <v>297</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="28" t="s">
-        <v>286</v>
+        <v>298</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="28" t="s">
-        <v>287</v>
+        <v>299</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="28" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="28" t="s">
-        <v>289</v>
+        <v>301</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="28" t="s">
-        <v>290</v>
+        <v>302</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="28" t="s">
-        <v>291</v>
+        <v>303</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="28" t="s">
-        <v>292</v>
+        <v>304</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="28" t="s">
-        <v>293</v>
+        <v>305</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="25" t="s">
-        <v>294</v>
+        <v>306</v>
       </c>
       <c r="B174" s="25"/>
       <c r="C174" s="25"/>
@@ -3831,7 +4053,7 @@
       <c r="G174" s="25"/>
       <c r="H174" s="25"/>
       <c r="I174" s="24" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3842,7 +4064,7 @@
       <c r="C175" s="29"/>
       <c r="D175" s="29"/>
       <c r="E175" s="27" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="F175" s="27"/>
       <c r="G175" s="27"/>
@@ -3850,57 +4072,57 @@
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="28" t="s">
-        <v>296</v>
+        <v>308</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="28" t="s">
-        <v>297</v>
+        <v>309</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="28" t="s">
-        <v>298</v>
+        <v>310</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="28" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="28" t="s">
-        <v>300</v>
+        <v>312</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="28" t="s">
-        <v>301</v>
+        <v>313</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="28" t="s">
-        <v>302</v>
+        <v>314</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="28" t="s">
-        <v>303</v>
+        <v>315</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="28" t="s">
-        <v>304</v>
+        <v>316</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="28" t="s">
-        <v>305</v>
+        <v>317</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="25" t="s">
-        <v>306</v>
+        <v>318</v>
       </c>
       <c r="B187" s="25"/>
       <c r="C187" s="25"/>
@@ -3910,18 +4132,18 @@
       <c r="G187" s="25"/>
       <c r="H187" s="25"/>
       <c r="I187" s="24" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A188" s="29" t="s">
-        <v>307</v>
+        <v>319</v>
       </c>
       <c r="B188" s="29"/>
       <c r="C188" s="29"/>
       <c r="D188" s="29"/>
       <c r="E188" s="27" t="s">
-        <v>308</v>
+        <v>320</v>
       </c>
       <c r="F188" s="27"/>
       <c r="G188" s="27"/>
@@ -3929,72 +4151,72 @@
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="28" t="s">
-        <v>309</v>
+        <v>321</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="28" t="s">
-        <v>310</v>
+        <v>322</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="28" t="s">
-        <v>311</v>
+        <v>323</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="28" t="s">
-        <v>312</v>
+        <v>324</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="28" t="s">
-        <v>313</v>
+        <v>325</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="28" t="s">
-        <v>314</v>
+        <v>326</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="28" t="s">
-        <v>315</v>
+        <v>327</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="28" t="s">
-        <v>316</v>
+        <v>328</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="28" t="s">
-        <v>317</v>
+        <v>329</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="28" t="s">
-        <v>318</v>
+        <v>330</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="28" t="s">
-        <v>319</v>
+        <v>331</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="28" t="s">
-        <v>320</v>
+        <v>332</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="28" t="s">
-        <v>321</v>
+        <v>333</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="25" t="s">
-        <v>322</v>
+        <v>334</v>
       </c>
       <c r="B203" s="25"/>
       <c r="C203" s="25"/>
@@ -4004,18 +4226,18 @@
       <c r="G203" s="25"/>
       <c r="H203" s="25"/>
       <c r="I203" s="24" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A204" s="29" t="s">
-        <v>323</v>
+        <v>335</v>
       </c>
       <c r="B204" s="29"/>
       <c r="C204" s="29"/>
       <c r="D204" s="29"/>
       <c r="E204" s="27" t="s">
-        <v>324</v>
+        <v>336</v>
       </c>
       <c r="F204" s="27"/>
       <c r="G204" s="27"/>
@@ -4023,82 +4245,82 @@
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="28" t="s">
-        <v>325</v>
+        <v>337</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="28" t="s">
-        <v>326</v>
+        <v>338</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="28" t="s">
-        <v>327</v>
+        <v>339</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="28" t="s">
-        <v>328</v>
+        <v>340</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="28" t="s">
-        <v>329</v>
+        <v>341</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="28" t="s">
-        <v>330</v>
+        <v>342</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="28" t="s">
-        <v>331</v>
+        <v>343</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="28" t="s">
-        <v>332</v>
+        <v>344</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="28" t="s">
-        <v>333</v>
+        <v>345</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="28" t="s">
-        <v>334</v>
+        <v>346</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="28" t="s">
-        <v>335</v>
+        <v>347</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="28" t="s">
-        <v>336</v>
+        <v>348</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="28" t="s">
-        <v>337</v>
+        <v>349</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="28" t="s">
-        <v>338</v>
+        <v>350</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="28" t="s">
-        <v>339</v>
+        <v>351</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="25" t="s">
-        <v>340</v>
+        <v>352</v>
       </c>
       <c r="B221" s="25"/>
       <c r="C221" s="25"/>
@@ -4107,86 +4329,312 @@
       <c r="F221" s="25"/>
       <c r="G221" s="25"/>
       <c r="H221" s="25"/>
-      <c r="I221" s="32" t="s">
-        <v>142</v>
+      <c r="I221" s="24" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A222" s="33" t="s">
+      <c r="A222" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="B222" s="33"/>
-      <c r="C222" s="33"/>
-      <c r="D222" s="33"/>
+      <c r="B222" s="29"/>
+      <c r="C222" s="29"/>
+      <c r="D222" s="29"/>
       <c r="E222" s="27" t="s">
-        <v>341</v>
+        <v>353</v>
       </c>
       <c r="F222" s="27"/>
       <c r="G222" s="27"/>
       <c r="H222" s="27"/>
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A223" s="34" t="s">
-        <v>342</v>
+      <c r="A223" s="28" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A224" s="34" t="s">
-        <v>343</v>
+      <c r="A224" s="28" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A225" s="34" t="s">
-        <v>344</v>
+      <c r="A225" s="28" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A226" s="34" t="s">
-        <v>345</v>
+      <c r="A226" s="28" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A227" s="34" t="s">
-        <v>346</v>
+      <c r="A227" s="28" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A228" s="34" t="s">
-        <v>347</v>
+      <c r="A228" s="28" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A229" s="34" t="s">
-        <v>348</v>
+      <c r="A229" s="28" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A230" s="34" t="s">
-        <v>349</v>
+      <c r="A230" s="28" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A231" s="34" t="s">
-        <v>350</v>
+      <c r="A231" s="28" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A232" s="34" t="s">
-        <v>351</v>
+      <c r="A232" s="28" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A233" s="34" t="s">
-        <v>352</v>
+      <c r="A233" s="28" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A234" s="34" t="s">
-        <v>353</v>
-      </c>
+      <c r="A234" s="28" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A236" s="25" t="s">
+        <v>366</v>
+      </c>
+      <c r="B236" s="25"/>
+      <c r="C236" s="25"/>
+      <c r="D236" s="25"/>
+      <c r="E236" s="25"/>
+      <c r="F236" s="25"/>
+      <c r="G236" s="25"/>
+      <c r="H236" s="25"/>
+      <c r="I236" s="24" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="237" customFormat="false" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A237" s="29" t="s">
+        <v>367</v>
+      </c>
+      <c r="B237" s="29"/>
+      <c r="C237" s="29"/>
+      <c r="D237" s="29"/>
+      <c r="E237" s="27" t="s">
+        <v>368</v>
+      </c>
+      <c r="F237" s="27"/>
+      <c r="G237" s="27"/>
+      <c r="H237" s="27"/>
+    </row>
+    <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A238" s="28" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A239" s="28" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A240" s="28" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A241" s="28" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A242" s="28" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A243" s="28" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A244" s="28" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A245" s="28" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A246" s="28" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A247" s="28" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A248" s="28" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A249" s="28" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A250" s="28" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A251" s="28" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A252" s="28" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A253" s="28" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A254" s="28" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A255" s="28" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A256" s="28" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A257" s="28" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A259" s="25" t="s">
+        <v>389</v>
+      </c>
+      <c r="B259" s="25"/>
+      <c r="C259" s="25"/>
+      <c r="D259" s="25"/>
+      <c r="E259" s="25"/>
+      <c r="F259" s="25"/>
+      <c r="G259" s="25"/>
+      <c r="H259" s="25"/>
+      <c r="I259" s="24" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="260" customFormat="false" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A260" s="29" t="s">
+        <v>390</v>
+      </c>
+      <c r="B260" s="29"/>
+      <c r="C260" s="29"/>
+      <c r="D260" s="29"/>
+      <c r="E260" s="27" t="s">
+        <v>391</v>
+      </c>
+      <c r="F260" s="27"/>
+      <c r="G260" s="27"/>
+      <c r="H260" s="27"/>
+    </row>
+    <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A261" s="28" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A262" s="32" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A263" s="32" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A264" s="32" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A265" s="32" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A266" s="32" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A267" s="32" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A268" s="32" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A269" s="32" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A270" s="32" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A271" s="32" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A272" s="32" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A273" s="32" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A274" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="45">
+  <mergeCells count="51">
     <mergeCell ref="A13:H13"/>
     <mergeCell ref="A14:D14"/>
     <mergeCell ref="E14:H14"/>
@@ -4232,6 +4680,12 @@
     <mergeCell ref="A221:H221"/>
     <mergeCell ref="A222:D222"/>
     <mergeCell ref="E222:H222"/>
+    <mergeCell ref="A236:H236"/>
+    <mergeCell ref="A237:D237"/>
+    <mergeCell ref="E237:H237"/>
+    <mergeCell ref="A259:H259"/>
+    <mergeCell ref="A260:D260"/>
+    <mergeCell ref="E260:H260"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="A13" display="1"/>
@@ -4249,6 +4703,8 @@
     <hyperlink ref="A2" location="A187" display="13"/>
     <hyperlink ref="B2" location="A203" display="14"/>
     <hyperlink ref="C2" location="A221" display="15"/>
+    <hyperlink ref="D2" location="A236" display="16"/>
+    <hyperlink ref="E2" location="A259" display="17"/>
     <hyperlink ref="I13" location="A1" display="Вверх"/>
     <hyperlink ref="I25" location="A1" display="Вверх"/>
     <hyperlink ref="I38" location="A1" display="Вверх"/>
@@ -4264,6 +4720,8 @@
     <hyperlink ref="I187" location="A1" display="Вверх"/>
     <hyperlink ref="I203" location="A1" display="Вверх"/>
     <hyperlink ref="I221" location="A1" display="Вверх"/>
+    <hyperlink ref="I236" location="A1" display="Вверх"/>
+    <hyperlink ref="I259" location="A1" display="Вверх"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
new docx file added
</commit_message>
<xml_diff>
--- a/psychology/CBT_new/mira.xlsx
+++ b/psychology/CBT_new/mira.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Искажения" sheetId="1" state="visible" r:id="rId3"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="430">
   <si>
     <t xml:space="preserve">№ позиции</t>
   </si>
@@ -831,6 +831,37 @@
 остаются незамеченными</t>
   </si>
   <si>
+    <t xml:space="preserve">Общение строится
+на обоюдных
+возможностях</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Общение со мной
+становится опасным</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Подруга жены эмоционально отстраняется
+в переписке после того, как я прямо
+высказал симпатию через комплименты</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Склонность интерпретировать поведение других людей
+через призму собственных эмоциональных реакций, что может
+приводить к поспешным выводам.
+2) Этот подход несёт риск усиления внутреннего напряжения и
+искажения восприятия отношений.
+3) Это может повлиять на мою уверенность и качество
+общения с окружающими.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">поведение других людей
+поспешные выводы
+внутреннее напряжение
+искажение восприятия
+уверенность
+качество общения</t>
+  </si>
+  <si>
     <t xml:space="preserve">1</t>
   </si>
   <si>
@@ -880,6 +911,9 @@
   </si>
   <si>
     <t xml:space="preserve">17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18</t>
   </si>
   <si>
     <t xml:space="preserve">Разбор 1 — Навешивание ярлыков | // моя работа по дому //</t>
@@ -1662,6 +1696,64 @@
   </si>
   <si>
     <t xml:space="preserve">13. Если вы теперь видите, что прогресс есть, даже в его малозаметных проявлениях, как это меняет ваше отношение к первоначальной мысли о том, что вы не видите своего прогресса и улучшения состояния?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Разборт 18 — Катастрофизация | // подруга отстраняется после моей симпатии //</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Общение со мной становится опасным</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Общение строится на обоюдных
+возможностях</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Скажите, какие доказательства у вас есть, что общение с вами действительно становится опасным?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. А есть ли какие-либо конкретные действия или слова с её стороны, которые прямо подтверждают, что она воспринимает ваши слова именно так?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Если она об этом не сообщала, то на чём тогда основано ваше убеждение, что она воспринимает это именно таким образом?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. А может ли быть какое-то другое объяснение её дистанции, помимо того, что она считает общение с вами опасным?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.  Если рассматривать эти возможные объяснения, как они меняют ваше восприятие её поведения?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6. Если ваше восприятие становится более спокойным при таких объяснениях, то насколько полезно для вас продолжать считать, что общение с вами становится опасным?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7. Если это бесполезно, то как вам кажется, что удерживало вас в этой мысли до сих пор?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8. Если теперь вы понимаете, что ваша интерпретация могла быть продиктована эмоциями, как вы могли бы взглянуть на эту ситуацию с более нейтральной точки зрения?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9. Если вы допускаете такие нейтральные объяснения, как это влияет на ваши чувства по отношению к её поведению?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10. Если злость уходит, как вам кажется, может ли эта ситуация быть не столько про «опасность общения», сколько про ваши ожидания и переживания?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11. Если это так, то как теперь вы оцениваете мысль «общение со мной становится опасным»? Насколько она кажется вам точной или полезной?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12. Если эта мысль неточна и бесполезна, как вам кажется, какой более гибкий и спокойный взгляд на ситуацию может вам сейчас подойти?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13. Если вы будете смотреть на ситуацию с этой точки зрения, что изменится в вашем восприятии и отношении к общению с ней?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14. Если вы будете относиться спокойнее, как это может повлиять на ваши дальнейшие мысли и чувства в подобных случаях?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15. Если ваши мысли станут менее эмоциональными, как вам кажется, будет ли легче поддерживать более тёплое и доверительное общение с другими?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16. Если вы видите, что более гибкий взгляд помогает вам сохранять спокойствие и улучшать общение, насколько теперь важно для вас отпускать прежние категоричные мысли в подобных ситуациях?</t>
   </si>
 </sst>
 </file>
@@ -2417,10 +2509,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H20" activeCellId="0" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2903,6 +2995,32 @@
         <v>13</v>
       </c>
     </row>
+    <row r="19" customFormat="false" ht="94.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="13" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="14" t="n">
+        <v>45639</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="G19" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="H19" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2919,10 +3037,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L274"/>
+  <dimension ref="A1:L292"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A255" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A293" activeCellId="0" sqref="A293"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2940,59 +3058,61 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="F1" s="24" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="G1" s="24" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="H1" s="24" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="I1" s="24" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="J1" s="24" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="K1" s="24" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="L1" s="24" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="24" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>152</v>
-      </c>
-      <c r="F2" s="24"/>
+        <v>157</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>158</v>
+      </c>
       <c r="G2" s="24"/>
       <c r="H2" s="24"/>
       <c r="I2" s="1"/>
@@ -3084,7 +3204,7 @@
     </row>
     <row r="13" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="25" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="B13" s="25"/>
       <c r="C13" s="25"/>
@@ -3094,7 +3214,7 @@
       <c r="G13" s="25"/>
       <c r="H13" s="25"/>
       <c r="I13" s="24" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3105,7 +3225,7 @@
       <c r="C14" s="26"/>
       <c r="D14" s="26"/>
       <c r="E14" s="27" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="F14" s="27"/>
       <c r="G14" s="27"/>
@@ -3113,52 +3233,52 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="28" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="28" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="28" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="28" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="28" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="28" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="28" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="28" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="28" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="25" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="B25" s="25"/>
       <c r="C25" s="25"/>
@@ -3168,18 +3288,18 @@
       <c r="G25" s="25"/>
       <c r="H25" s="25"/>
       <c r="I25" s="24" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="26" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="B26" s="26"/>
       <c r="C26" s="26"/>
       <c r="D26" s="26"/>
       <c r="E26" s="27" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="F26" s="27"/>
       <c r="G26" s="27"/>
@@ -3187,57 +3307,57 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="28" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="28" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="28" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="28" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="28" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="28" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="28" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="28" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="28" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="28" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="25" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="B38" s="25"/>
       <c r="C38" s="25"/>
@@ -3247,18 +3367,18 @@
       <c r="G38" s="25"/>
       <c r="H38" s="25"/>
       <c r="I38" s="24" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="29" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="B39" s="29"/>
       <c r="C39" s="29"/>
       <c r="D39" s="29"/>
       <c r="E39" s="27" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="F39" s="27"/>
       <c r="G39" s="27"/>
@@ -3266,77 +3386,77 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="28" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="28" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="28" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="28" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="28" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="28" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="28" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="28" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="28" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="28" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="28" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="28" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="28" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="28" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="25" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="B55" s="25"/>
       <c r="C55" s="25"/>
@@ -3346,18 +3466,18 @@
       <c r="G55" s="25"/>
       <c r="H55" s="25"/>
       <c r="I55" s="24" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="52.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="29" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="B56" s="29"/>
       <c r="C56" s="29"/>
       <c r="D56" s="29"/>
       <c r="E56" s="27" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="F56" s="27"/>
       <c r="G56" s="27"/>
@@ -3365,62 +3485,62 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="28" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="28" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="28" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="28" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="28" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="28" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="28" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="28" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="28" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="28" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="28" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="25" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="B69" s="25"/>
       <c r="C69" s="25"/>
@@ -3430,7 +3550,7 @@
       <c r="G69" s="25"/>
       <c r="H69" s="25"/>
       <c r="I69" s="24" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="36.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3441,7 +3561,7 @@
       <c r="C70" s="29"/>
       <c r="D70" s="29"/>
       <c r="E70" s="27" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="F70" s="27"/>
       <c r="G70" s="27"/>
@@ -3449,62 +3569,62 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="28" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="28" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="28" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="28" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="28" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="30" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="28" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="28" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="28" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="28" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="28" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="25" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="B83" s="25"/>
       <c r="C83" s="25"/>
@@ -3514,7 +3634,7 @@
       <c r="G83" s="25"/>
       <c r="H83" s="25"/>
       <c r="I83" s="24" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3525,7 +3645,7 @@
       <c r="C84" s="29"/>
       <c r="D84" s="29"/>
       <c r="E84" s="27" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="F84" s="27"/>
       <c r="G84" s="27"/>
@@ -3533,52 +3653,52 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="28" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="28" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="28" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="28" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="28" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="28" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="28" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="28" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="28" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="25" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="B95" s="25"/>
       <c r="C95" s="25"/>
@@ -3588,7 +3708,7 @@
       <c r="G95" s="25"/>
       <c r="H95" s="25"/>
       <c r="I95" s="24" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="19.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3607,62 +3727,62 @@
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="28" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="28" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="28" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="28" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="28" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="28" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="28" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="28" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="28" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="28" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="28" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="25" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="B109" s="25"/>
       <c r="C109" s="25"/>
@@ -3672,7 +3792,7 @@
       <c r="G109" s="25"/>
       <c r="H109" s="25"/>
       <c r="I109" s="24" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="27.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3683,7 +3803,7 @@
       <c r="C110" s="31"/>
       <c r="D110" s="31"/>
       <c r="E110" s="27" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="F110" s="27"/>
       <c r="G110" s="27"/>
@@ -3691,62 +3811,62 @@
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="28" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="28" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="28" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="28" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="28" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="28" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="28" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="28" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="28" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="28" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="28" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="25" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="B123" s="25"/>
       <c r="C123" s="25"/>
@@ -3756,7 +3876,7 @@
       <c r="G123" s="25"/>
       <c r="H123" s="25"/>
       <c r="I123" s="24" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3767,7 +3887,7 @@
       <c r="C124" s="29"/>
       <c r="D124" s="29"/>
       <c r="E124" s="27" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="F124" s="27"/>
       <c r="G124" s="27"/>
@@ -3775,77 +3895,77 @@
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="28" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="28" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="28" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="28" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="28" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="28" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="28" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="28" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="28" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="28" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="28" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="28" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="28" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="28" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="25" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="B140" s="25"/>
       <c r="C140" s="25"/>
@@ -3855,7 +3975,7 @@
       <c r="G140" s="25"/>
       <c r="H140" s="25"/>
       <c r="I140" s="24" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3866,7 +3986,7 @@
       <c r="C141" s="29"/>
       <c r="D141" s="29"/>
       <c r="E141" s="27" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="F141" s="27"/>
       <c r="G141" s="27"/>
@@ -3874,82 +3994,82 @@
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="28" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="28" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="28" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="28" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="28" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="28" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="28" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="28" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="28" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="28" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="28" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="28" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="28" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="28" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="28" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="25" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
       <c r="B158" s="25"/>
       <c r="C158" s="25"/>
@@ -3959,7 +4079,7 @@
       <c r="G158" s="25"/>
       <c r="H158" s="25"/>
       <c r="I158" s="24" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3970,7 +4090,7 @@
       <c r="C159" s="29"/>
       <c r="D159" s="29"/>
       <c r="E159" s="27" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
       <c r="F159" s="27"/>
       <c r="G159" s="27"/>
@@ -3978,72 +4098,72 @@
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="28" t="s">
-        <v>293</v>
+        <v>299</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="28" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="28" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="28" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="28" t="s">
-        <v>297</v>
+        <v>303</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="28" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="28" t="s">
-        <v>299</v>
+        <v>305</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="28" t="s">
-        <v>300</v>
+        <v>306</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="28" t="s">
-        <v>301</v>
+        <v>307</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="28" t="s">
-        <v>302</v>
+        <v>308</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="28" t="s">
-        <v>303</v>
+        <v>309</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="28" t="s">
-        <v>304</v>
+        <v>310</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="28" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="25" t="s">
-        <v>306</v>
+        <v>312</v>
       </c>
       <c r="B174" s="25"/>
       <c r="C174" s="25"/>
@@ -4053,7 +4173,7 @@
       <c r="G174" s="25"/>
       <c r="H174" s="25"/>
       <c r="I174" s="24" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4064,7 +4184,7 @@
       <c r="C175" s="29"/>
       <c r="D175" s="29"/>
       <c r="E175" s="27" t="s">
-        <v>307</v>
+        <v>313</v>
       </c>
       <c r="F175" s="27"/>
       <c r="G175" s="27"/>
@@ -4072,57 +4192,57 @@
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="28" t="s">
-        <v>308</v>
+        <v>314</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="28" t="s">
-        <v>309</v>
+        <v>315</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="28" t="s">
-        <v>310</v>
+        <v>316</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="28" t="s">
-        <v>311</v>
+        <v>317</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="28" t="s">
-        <v>312</v>
+        <v>318</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="28" t="s">
-        <v>313</v>
+        <v>319</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="28" t="s">
-        <v>314</v>
+        <v>320</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="28" t="s">
-        <v>315</v>
+        <v>321</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="28" t="s">
-        <v>316</v>
+        <v>322</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="28" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="25" t="s">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="B187" s="25"/>
       <c r="C187" s="25"/>
@@ -4132,18 +4252,18 @@
       <c r="G187" s="25"/>
       <c r="H187" s="25"/>
       <c r="I187" s="24" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A188" s="29" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="B188" s="29"/>
       <c r="C188" s="29"/>
       <c r="D188" s="29"/>
       <c r="E188" s="27" t="s">
-        <v>320</v>
+        <v>326</v>
       </c>
       <c r="F188" s="27"/>
       <c r="G188" s="27"/>
@@ -4151,72 +4271,72 @@
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="28" t="s">
-        <v>321</v>
+        <v>327</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="28" t="s">
-        <v>322</v>
+        <v>328</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="28" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="28" t="s">
-        <v>324</v>
+        <v>330</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="28" t="s">
-        <v>325</v>
+        <v>331</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="28" t="s">
-        <v>326</v>
+        <v>332</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="28" t="s">
-        <v>327</v>
+        <v>333</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="28" t="s">
-        <v>328</v>
+        <v>334</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="28" t="s">
-        <v>329</v>
+        <v>335</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="28" t="s">
-        <v>330</v>
+        <v>336</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="28" t="s">
-        <v>331</v>
+        <v>337</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="28" t="s">
-        <v>332</v>
+        <v>338</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="28" t="s">
-        <v>333</v>
+        <v>339</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="25" t="s">
-        <v>334</v>
+        <v>340</v>
       </c>
       <c r="B203" s="25"/>
       <c r="C203" s="25"/>
@@ -4226,18 +4346,18 @@
       <c r="G203" s="25"/>
       <c r="H203" s="25"/>
       <c r="I203" s="24" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A204" s="29" t="s">
-        <v>335</v>
+        <v>341</v>
       </c>
       <c r="B204" s="29"/>
       <c r="C204" s="29"/>
       <c r="D204" s="29"/>
       <c r="E204" s="27" t="s">
-        <v>336</v>
+        <v>342</v>
       </c>
       <c r="F204" s="27"/>
       <c r="G204" s="27"/>
@@ -4245,82 +4365,82 @@
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="28" t="s">
-        <v>337</v>
+        <v>343</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="28" t="s">
-        <v>338</v>
+        <v>344</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="28" t="s">
-        <v>339</v>
+        <v>345</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="28" t="s">
-        <v>340</v>
+        <v>346</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="28" t="s">
-        <v>341</v>
+        <v>347</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="28" t="s">
-        <v>342</v>
+        <v>348</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="28" t="s">
-        <v>343</v>
+        <v>349</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="28" t="s">
-        <v>344</v>
+        <v>350</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="28" t="s">
-        <v>345</v>
+        <v>351</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="28" t="s">
-        <v>346</v>
+        <v>352</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="28" t="s">
-        <v>347</v>
+        <v>353</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="28" t="s">
-        <v>348</v>
+        <v>354</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="28" t="s">
-        <v>349</v>
+        <v>355</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="28" t="s">
-        <v>350</v>
+        <v>356</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="28" t="s">
-        <v>351</v>
+        <v>357</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="25" t="s">
-        <v>352</v>
+        <v>358</v>
       </c>
       <c r="B221" s="25"/>
       <c r="C221" s="25"/>
@@ -4330,7 +4450,7 @@
       <c r="G221" s="25"/>
       <c r="H221" s="25"/>
       <c r="I221" s="24" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4341,7 +4461,7 @@
       <c r="C222" s="29"/>
       <c r="D222" s="29"/>
       <c r="E222" s="27" t="s">
-        <v>353</v>
+        <v>359</v>
       </c>
       <c r="F222" s="27"/>
       <c r="G222" s="27"/>
@@ -4349,67 +4469,67 @@
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="28" t="s">
-        <v>354</v>
+        <v>360</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="28" t="s">
-        <v>355</v>
+        <v>361</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="28" t="s">
-        <v>356</v>
+        <v>362</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="28" t="s">
-        <v>357</v>
+        <v>363</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="28" t="s">
-        <v>358</v>
+        <v>364</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="28" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="28" t="s">
-        <v>360</v>
+        <v>366</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="28" t="s">
-        <v>361</v>
+        <v>367</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="28" t="s">
-        <v>362</v>
+        <v>368</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="28" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="28" t="s">
-        <v>364</v>
+        <v>370</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="28" t="s">
-        <v>365</v>
+        <v>371</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="25" t="s">
-        <v>366</v>
+        <v>372</v>
       </c>
       <c r="B236" s="25"/>
       <c r="C236" s="25"/>
@@ -4419,18 +4539,18 @@
       <c r="G236" s="25"/>
       <c r="H236" s="25"/>
       <c r="I236" s="24" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A237" s="29" t="s">
-        <v>367</v>
+        <v>373</v>
       </c>
       <c r="B237" s="29"/>
       <c r="C237" s="29"/>
       <c r="D237" s="29"/>
       <c r="E237" s="27" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="F237" s="27"/>
       <c r="G237" s="27"/>
@@ -4438,107 +4558,107 @@
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="28" t="s">
-        <v>369</v>
+        <v>375</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="28" t="s">
-        <v>370</v>
+        <v>376</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="28" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="28" t="s">
-        <v>372</v>
+        <v>378</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="28" t="s">
-        <v>373</v>
+        <v>379</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="28" t="s">
-        <v>374</v>
+        <v>380</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="28" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="28" t="s">
-        <v>376</v>
+        <v>382</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="28" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="28" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="28" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="28" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="28" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="28" t="s">
-        <v>382</v>
+        <v>388</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="28" t="s">
-        <v>383</v>
+        <v>389</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="28" t="s">
-        <v>384</v>
+        <v>390</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="28" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="28" t="s">
-        <v>386</v>
+        <v>392</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="28" t="s">
-        <v>387</v>
+        <v>393</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="28" t="s">
-        <v>388</v>
+        <v>394</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="25" t="s">
-        <v>389</v>
+        <v>395</v>
       </c>
       <c r="B259" s="25"/>
       <c r="C259" s="25"/>
@@ -4548,18 +4668,18 @@
       <c r="G259" s="25"/>
       <c r="H259" s="25"/>
       <c r="I259" s="24" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A260" s="29" t="s">
-        <v>390</v>
+        <v>396</v>
       </c>
       <c r="B260" s="29"/>
       <c r="C260" s="29"/>
       <c r="D260" s="29"/>
       <c r="E260" s="27" t="s">
-        <v>391</v>
+        <v>397</v>
       </c>
       <c r="F260" s="27"/>
       <c r="G260" s="27"/>
@@ -4567,74 +4687,183 @@
     </row>
     <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="28" t="s">
-        <v>392</v>
+        <v>398</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A262" s="32" t="s">
-        <v>393</v>
+      <c r="A262" s="28" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A263" s="32" t="s">
-        <v>394</v>
+      <c r="A263" s="28" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A264" s="32" t="s">
-        <v>395</v>
+      <c r="A264" s="28" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A265" s="32" t="s">
-        <v>396</v>
+      <c r="A265" s="28" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A266" s="32" t="s">
-        <v>397</v>
+      <c r="A266" s="28" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A267" s="32" t="s">
-        <v>398</v>
+      <c r="A267" s="28" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A268" s="32" t="s">
-        <v>399</v>
+      <c r="A268" s="28" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A269" s="32" t="s">
-        <v>400</v>
+      <c r="A269" s="28" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A270" s="32" t="s">
-        <v>401</v>
+      <c r="A270" s="28" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A271" s="32" t="s">
-        <v>402</v>
+      <c r="A271" s="28" t="s">
+        <v>408</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A272" s="32" t="s">
-        <v>403</v>
+      <c r="A272" s="28" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A273" s="32" t="s">
-        <v>404</v>
+      <c r="A273" s="28" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="28"/>
     </row>
+    <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A275" s="25" t="s">
+        <v>411</v>
+      </c>
+      <c r="B275" s="25"/>
+      <c r="C275" s="25"/>
+      <c r="D275" s="25"/>
+      <c r="E275" s="25"/>
+      <c r="F275" s="25"/>
+      <c r="G275" s="25"/>
+      <c r="H275" s="25"/>
+      <c r="I275" s="24" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="276" customFormat="false" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A276" s="29" t="s">
+        <v>412</v>
+      </c>
+      <c r="B276" s="29"/>
+      <c r="C276" s="29"/>
+      <c r="D276" s="29"/>
+      <c r="E276" s="27" t="s">
+        <v>413</v>
+      </c>
+      <c r="F276" s="27"/>
+      <c r="G276" s="27"/>
+      <c r="H276" s="27"/>
+    </row>
+    <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A277" s="32" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A278" s="32" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A279" s="32" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A280" s="32" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A281" s="32" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A282" s="32" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A283" s="32" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A284" s="32" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A285" s="32" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A286" s="32" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A287" s="32" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A288" s="32" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A289" s="32" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A290" s="32" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A291" s="32" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A292" s="32" t="s">
+        <v>429</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="51">
+  <mergeCells count="54">
     <mergeCell ref="A13:H13"/>
     <mergeCell ref="A14:D14"/>
     <mergeCell ref="E14:H14"/>
@@ -4686,6 +4915,9 @@
     <mergeCell ref="A259:H259"/>
     <mergeCell ref="A260:D260"/>
     <mergeCell ref="E260:H260"/>
+    <mergeCell ref="A275:H275"/>
+    <mergeCell ref="A276:D276"/>
+    <mergeCell ref="E276:H276"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="A13" display="1"/>
@@ -4705,6 +4937,7 @@
     <hyperlink ref="C2" location="A221" display="15"/>
     <hyperlink ref="D2" location="A236" display="16"/>
     <hyperlink ref="E2" location="A259" display="17"/>
+    <hyperlink ref="F2" location="A275" display="18"/>
     <hyperlink ref="I13" location="A1" display="Вверх"/>
     <hyperlink ref="I25" location="A1" display="Вверх"/>
     <hyperlink ref="I38" location="A1" display="Вверх"/>
@@ -4722,6 +4955,7 @@
     <hyperlink ref="I221" location="A1" display="Вверх"/>
     <hyperlink ref="I236" location="A1" display="Вверх"/>
     <hyperlink ref="I259" location="A1" display="Вверх"/>
+    <hyperlink ref="I275" location="A1" display="Вверх"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>